<commit_message>
can do some basic predictions now
</commit_message>
<xml_diff>
--- a/tyrewear.xlsx
+++ b/tyrewear.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="100" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="37">
   <si>
     <t>name</t>
   </si>
@@ -126,13 +126,7 @@
     <t>soft_slope</t>
   </si>
   <si>
-    <t>soft_int</t>
-  </si>
-  <si>
     <t>hard_slope</t>
-  </si>
-  <si>
-    <t>hard_int</t>
   </si>
 </sst>
 </file>
@@ -481,21 +475,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P18"/>
+  <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+      <selection activeCell="I12" sqref="I12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="8" max="8" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.5546875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="10" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="9.5546875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -524,25 +518,13 @@
         <v>36</v>
       </c>
       <c r="J1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="K1" t="s">
-        <v>38</v>
-      </c>
-      <c r="L1" t="s">
-        <v>35</v>
-      </c>
-      <c r="M1" t="s">
         <v>36</v>
       </c>
-      <c r="N1" t="s">
-        <v>37</v>
-      </c>
-      <c r="O1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -565,7 +547,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>11</v>
       </c>
@@ -588,7 +570,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -611,39 +593,25 @@
         <v>13</v>
       </c>
       <c r="H4">
-        <v>-0.78569999999999995</v>
+        <v>-8.76</v>
       </c>
       <c r="I4">
-        <v>11.856999999999999</v>
+        <v>-4.59</v>
       </c>
       <c r="J4">
-        <v>-0.16969999999999999</v>
+        <f>H4/B4</f>
+        <v>-1.6070445789763348</v>
       </c>
       <c r="K4">
-        <v>5.5332999999999997</v>
-      </c>
-      <c r="L4">
-        <f>H4/B4</f>
-        <v>-0.14413869014859659</v>
-      </c>
-      <c r="M4">
         <f>I4/B4</f>
-        <v>2.175197211520822</v>
-      </c>
-      <c r="N4">
-        <f>J4/B4</f>
-        <v>-3.1131902403228766E-2</v>
-      </c>
-      <c r="O4">
-        <f>K4/B4</f>
-        <v>1.0150981471289671</v>
-      </c>
-      <c r="P4" t="str">
-        <f t="shared" ref="P4:P10" si="0">G4</f>
+        <v>-0.84204733076499727</v>
+      </c>
+      <c r="L4" t="str">
+        <f>G4</f>
         <v>vhigh</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>16</v>
       </c>
@@ -666,39 +634,25 @@
         <v>12</v>
       </c>
       <c r="H5">
-        <v>-3.5700000000000003E-2</v>
+        <v>-10.25</v>
       </c>
       <c r="I5">
-        <v>10.286</v>
+        <v>-6.34</v>
       </c>
       <c r="J5">
-        <v>-0.16039999999999999</v>
+        <f>H5/B5</f>
+        <v>-1.893939393939394</v>
       </c>
       <c r="K5">
-        <v>7.1318999999999999</v>
-      </c>
-      <c r="L5">
-        <f>H5/B5</f>
-        <v>-6.5964523281596462E-3</v>
-      </c>
-      <c r="M5">
         <f>I5/B5</f>
-        <v>1.9005912786400592</v>
-      </c>
-      <c r="N5">
-        <f t="shared" ref="N5:N10" si="1">J5/B5</f>
-        <v>-2.9637841832963783E-2</v>
-      </c>
-      <c r="O5">
-        <f t="shared" ref="O5:O10" si="2">K5/B5</f>
-        <v>1.3177937915742794</v>
-      </c>
-      <c r="P5" t="str">
-        <f t="shared" si="0"/>
+        <v>-1.171470805617147</v>
+      </c>
+      <c r="L5" t="str">
+        <f>G5</f>
         <v>high</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>17</v>
       </c>
@@ -721,39 +675,25 @@
         <v>13</v>
       </c>
       <c r="H6">
-        <v>-0.6</v>
+        <v>-9</v>
       </c>
       <c r="I6">
-        <v>10.5</v>
+        <v>-4.22</v>
       </c>
       <c r="J6">
-        <v>-0.15759999999999999</v>
+        <f>H6/B6</f>
+        <v>-1.9334049409237377</v>
       </c>
       <c r="K6">
-        <v>5.0667</v>
-      </c>
-      <c r="L6">
-        <f t="shared" ref="L6:L10" si="3">H6/B6</f>
-        <v>-0.12889366272824918</v>
-      </c>
-      <c r="M6">
-        <f t="shared" ref="M6:M10" si="4">I6/B6</f>
-        <v>2.255639097744361</v>
-      </c>
-      <c r="N6">
-        <f t="shared" si="1"/>
-        <v>-3.3856068743286782E-2</v>
-      </c>
-      <c r="O6">
-        <f t="shared" si="2"/>
-        <v>1.0884425349087004</v>
-      </c>
-      <c r="P6" t="str">
-        <f t="shared" si="0"/>
+        <f>I6/B6</f>
+        <v>-0.90655209452201924</v>
+      </c>
+      <c r="L6" t="str">
+        <f>G6</f>
         <v>vhigh</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>18</v>
       </c>
@@ -776,33 +716,22 @@
         <v>20</v>
       </c>
       <c r="H7">
-        <v>-0.17269999999999999</v>
-      </c>
-      <c r="I7">
-        <v>5.1273</v>
-      </c>
-      <c r="L7">
-        <f t="shared" si="3"/>
-        <v>-5.1706586826347302E-2</v>
-      </c>
-      <c r="M7">
-        <f t="shared" si="4"/>
-        <v>1.5351197604790419</v>
-      </c>
-      <c r="N7">
-        <f t="shared" si="1"/>
+        <v>-4.0869999999999997</v>
+      </c>
+      <c r="J7">
+        <f>H7/B7</f>
+        <v>-1.2236526946107784</v>
+      </c>
+      <c r="K7">
+        <f>I7/B7</f>
         <v>0</v>
       </c>
-      <c r="O7">
-        <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="P7" t="str">
-        <f t="shared" si="0"/>
+      <c r="L7" t="str">
+        <f>G7</f>
         <v>low</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>21</v>
       </c>
@@ -825,39 +754,25 @@
         <v>13</v>
       </c>
       <c r="H8">
-        <v>-0.8286</v>
+        <v>-9.5</v>
       </c>
       <c r="I8">
-        <v>12.4</v>
+        <v>-4.9000000000000004</v>
       </c>
       <c r="J8">
-        <v>-0.2</v>
+        <f>H8/B8</f>
+        <v>-1.7796927688272761</v>
       </c>
       <c r="K8">
-        <v>6</v>
-      </c>
-      <c r="L8">
-        <f t="shared" si="3"/>
-        <v>-0.15522667665792431</v>
-      </c>
-      <c r="M8">
-        <f t="shared" si="4"/>
-        <v>2.3229674035219183</v>
-      </c>
-      <c r="N8">
-        <f t="shared" si="1"/>
-        <v>-3.7467216185837392E-2</v>
-      </c>
-      <c r="O8">
-        <f t="shared" si="2"/>
-        <v>1.1240164855751218</v>
-      </c>
-      <c r="P8" t="str">
-        <f t="shared" si="0"/>
+        <f>I8/B8</f>
+        <v>-0.91794679655301614</v>
+      </c>
+      <c r="L8" t="str">
+        <f>G8</f>
         <v>vhigh</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -880,39 +795,25 @@
         <v>10</v>
       </c>
       <c r="H9">
-        <v>-0.35</v>
+        <v>-7.96</v>
       </c>
       <c r="I9">
-        <v>9.1999999999999993</v>
+        <v>-3.81</v>
       </c>
       <c r="J9">
-        <v>-4.5499999999999999E-2</v>
+        <f>H9/B9</f>
+        <v>-1.5483368994359075</v>
       </c>
       <c r="K9">
-        <v>4.0909000000000004</v>
-      </c>
-      <c r="L9">
-        <f t="shared" si="3"/>
-        <v>-6.808014005057382E-2</v>
-      </c>
-      <c r="M9">
-        <f t="shared" si="4"/>
-        <v>1.7895351099007974</v>
-      </c>
-      <c r="N9">
-        <f t="shared" si="1"/>
-        <v>-8.8504182065745965E-3</v>
-      </c>
-      <c r="O9">
-        <f t="shared" si="2"/>
-        <v>0.79574012837969277</v>
-      </c>
-      <c r="P9" t="str">
-        <f t="shared" si="0"/>
+        <f>I9/B9</f>
+        <v>-0.74110095312196067</v>
+      </c>
+      <c r="L9" t="str">
+        <f>G9</f>
         <v>avg</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>23</v>
       </c>
@@ -935,39 +836,25 @@
         <v>10</v>
       </c>
       <c r="H10">
-        <v>-0.7</v>
+        <v>-7.91</v>
       </c>
       <c r="I10">
-        <v>10.1</v>
+        <v>-3.7450000000000001</v>
       </c>
       <c r="J10">
-        <v>-8.1799999999999998E-2</v>
+        <f>H10/B10</f>
+        <v>-1.5365190365190367</v>
       </c>
       <c r="K10">
-        <v>4.2182000000000004</v>
-      </c>
-      <c r="L10">
-        <f t="shared" si="3"/>
-        <v>-0.13597513597513597</v>
-      </c>
-      <c r="M10">
-        <f t="shared" si="4"/>
-        <v>1.9619269619269619</v>
-      </c>
-      <c r="N10">
-        <f t="shared" si="1"/>
-        <v>-1.588966588966589E-2</v>
-      </c>
-      <c r="O10">
-        <f t="shared" si="2"/>
-        <v>0.81938616938616948</v>
-      </c>
-      <c r="P10" t="str">
-        <f t="shared" si="0"/>
+        <f>I10/B10</f>
+        <v>-0.72746697746697753</v>
+      </c>
+      <c r="L10" t="str">
+        <f>G10</f>
         <v>avg</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>24</v>
       </c>
@@ -989,8 +876,25 @@
       <c r="G11" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="H11">
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <v>-2.39</v>
+      </c>
+      <c r="J11">
+        <f>H11/B11</f>
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <f>I11/B11</f>
+        <v>-0.54553754850490754</v>
+      </c>
+      <c r="L11" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>25</v>
       </c>
@@ -1013,7 +917,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>26</v>
       </c>
@@ -1036,7 +940,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>27</v>
       </c>
@@ -1059,7 +963,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>29</v>
       </c>
@@ -1081,9 +985,9 @@
       <c r="G15" t="s">
         <v>10</v>
       </c>
-      <c r="N15" s="1"/>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="K15" s="1"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>31</v>
       </c>
@@ -1105,7 +1009,6 @@
       <c r="G16" t="s">
         <v>12</v>
       </c>
-      <c r="K16" s="1"/>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A17" t="s">

</xml_diff>